<commit_message>
Deletion of output files before starting code and type of node in car schedule output added
</commit_message>
<xml_diff>
--- a/data/data_2.xlsx
+++ b/data/data_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/falkzimmer/Desktop/UNI/01_Master/01_Semester/03/Projektmodul/00 PM Coding /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/falkzimmer/Desktop/UNI/01_Master/01_Semester/03/Projektmodul/00 PM Coding  piecewise/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C3B5B-4EA8-A749-AE4C-0BEFC0F8AA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B500F324-652A-174A-B0BD-DA18DF14D922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{5ED0D196-DC63-0A40-9FF8-A9B38A6CE3F7}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +514,7 @@
         <v>630</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>30</v>

</xml_diff>